<commit_message>
Refactor StatusIndicator: updated layout margins, replaced custom status light with a simple circle label, and improved text styling. Adjusted stylesheet for consistent appearance and enhanced visual clarity.
</commit_message>
<xml_diff>
--- a/Zips by Address File Group.xlsx
+++ b/Zips by Address File Group.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimelj/WebDev/CBA/mailApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596FF37A-6952-3C4F-BDCD-9137665FAC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DF749B-4552-D840-BC57-1DC47618E1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31220" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{FF0AFF27-4EB4-4517-B714-952991B7B0BD}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{FF0AFF27-4EB4-4517-B714-952991B7B0BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="9" r:id="rId1"/>
@@ -36,47 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="32">
-  <si>
-    <t>CBAW5</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="36">
   <si>
     <t>DDU</t>
   </si>
   <si>
-    <t>CBAW12</t>
-  </si>
-  <si>
     <t>CBAT5</t>
   </si>
   <si>
-    <t>CBAW3</t>
-  </si>
-  <si>
-    <t>CBAW9</t>
-  </si>
-  <si>
-    <t>CBAW11</t>
-  </si>
-  <si>
-    <t>CBAW6</t>
-  </si>
-  <si>
-    <t>CBAW8</t>
-  </si>
-  <si>
-    <t>CBAW10</t>
-  </si>
-  <si>
     <t>CBAT7</t>
   </si>
   <si>
-    <t>CBAW7</t>
-  </si>
-  <si>
-    <t>CBATW1</t>
-  </si>
-  <si>
     <t>CBAT3</t>
   </si>
   <si>
@@ -86,9 +56,6 @@
     <t>CBAT1</t>
   </si>
   <si>
-    <t>CBAW1</t>
-  </si>
-  <si>
     <t>CBAT99</t>
   </si>
   <si>
@@ -98,18 +65,12 @@
     <t>CBAT4</t>
   </si>
   <si>
-    <t>CBAW2</t>
-  </si>
-  <si>
     <t>CBAT9</t>
   </si>
   <si>
     <t>CBAT6</t>
   </si>
   <si>
-    <t>CBAW4</t>
-  </si>
-  <si>
     <t>CBAT2</t>
   </si>
   <si>
@@ -128,10 +89,61 @@
     <t>TUE</t>
   </si>
   <si>
-    <t>WED</t>
-  </si>
-  <si>
     <t>CBAT10</t>
+  </si>
+  <si>
+    <t>MON</t>
+  </si>
+  <si>
+    <t>CBAM5</t>
+  </si>
+  <si>
+    <t>CBAM1</t>
+  </si>
+  <si>
+    <t>CBAM10</t>
+  </si>
+  <si>
+    <t>CBAM2</t>
+  </si>
+  <si>
+    <t>CBAM3</t>
+  </si>
+  <si>
+    <t>CBAM4</t>
+  </si>
+  <si>
+    <t>CBAM6</t>
+  </si>
+  <si>
+    <t>CBAM7</t>
+  </si>
+  <si>
+    <t>CBAM8</t>
+  </si>
+  <si>
+    <t>CBAM9</t>
+  </si>
+  <si>
+    <t>CBAMT1-1</t>
+  </si>
+  <si>
+    <t>CBAMT1-2</t>
+  </si>
+  <si>
+    <t>CBAMT1-3</t>
+  </si>
+  <si>
+    <t>CBAMT1-4</t>
+  </si>
+  <si>
+    <t>CBAMT1-5</t>
+  </si>
+  <si>
+    <t>CBAT11</t>
+  </si>
+  <si>
+    <t>CBAT12</t>
   </si>
 </sst>
 </file>
@@ -173,7 +185,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -516,329 +538,329 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC217B0-B495-4842-AF2B-3B0E925991E5}">
   <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>11020</v>
+        <v>11703</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>11021</v>
+        <v>11729</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>11023</v>
+        <v>11795</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>11024</v>
+        <v>11798</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>11040</v>
+        <v>11720</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>11501</v>
+        <v>11733</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>11507</v>
+        <v>11776</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>11530</v>
+        <v>11777</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>11566</v>
+        <v>11787</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>11596</v>
+        <v>11788</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11701</v>
+        <v>11790</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11702</v>
+        <v>11758</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>11703</v>
+        <v>11783</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>11704</v>
+        <v>11701</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>11710</v>
+        <v>11726</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>11717</v>
+        <v>11757</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>11721</v>
+        <v>11717</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>11724</v>
+        <v>11730</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>11725</v>
+        <v>11735</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>11726</v>
+        <v>11751</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>11729</v>
+        <v>11752</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>11730</v>
+        <v>11020</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
         <v>19</v>
@@ -846,41 +868,41 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>11731</v>
+        <v>11021</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>11733</v>
+        <v>11023</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>11735</v>
+        <v>11024</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
         <v>19</v>
@@ -888,41 +910,41 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>11740</v>
+        <v>11040</v>
       </c>
       <c r="B27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>11743</v>
+        <v>11501</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>11751</v>
+        <v>11507</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
         <v>19</v>
@@ -930,13 +952,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>11752</v>
+        <v>11530</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D30" t="s">
         <v>19</v>
@@ -944,1273 +966,1273 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>11754</v>
+        <v>11596</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>11757</v>
+        <v>11725</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>11758</v>
+        <v>11731</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>11762</v>
+        <v>11754</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>11768</v>
+        <v>11566</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>11776</v>
+        <v>11710</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>11777</v>
+        <v>11793</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>11783</v>
+        <v>11702</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>11787</v>
+        <v>11704</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>11788</v>
+        <v>11762</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>11790</v>
+        <v>11721</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>11793</v>
+        <v>11724</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>11795</v>
+        <v>11740</v>
       </c>
       <c r="B43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>11798</v>
+        <v>11743</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>11713</v>
+        <v>11768</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>11719</v>
+        <v>11803</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>11764</v>
+        <v>11713</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>11778</v>
+        <v>11719</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>11786</v>
+        <v>11764</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>11789</v>
+        <v>11778</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>11792</v>
+        <v>11786</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>11901</v>
+        <v>11789</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>11933</v>
+        <v>11792</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>11934</v>
+        <v>11901</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D54" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>11935</v>
+        <v>11933</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>11937</v>
+        <v>11934</v>
       </c>
       <c r="B56" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>11939</v>
+        <v>11935</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D57" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>11940</v>
+        <v>11937</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D58" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>11941</v>
+        <v>11939</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>11942</v>
+        <v>11940</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>11944</v>
+        <v>11941</v>
       </c>
       <c r="B61" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D61" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>11946</v>
+        <v>11942</v>
       </c>
       <c r="B62" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>11948</v>
+        <v>11944</v>
       </c>
       <c r="B63" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D63" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>11949</v>
+        <v>11946</v>
       </c>
       <c r="B64" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D64" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>11950</v>
+        <v>11948</v>
       </c>
       <c r="B65" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D65" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>11951</v>
+        <v>11949</v>
       </c>
       <c r="B66" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D66" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>11952</v>
+        <v>11950</v>
       </c>
       <c r="B67" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D67" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>11953</v>
+        <v>11951</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D68" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>11954</v>
+        <v>11952</v>
       </c>
       <c r="B69" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>11955</v>
+        <v>11953</v>
       </c>
       <c r="B70" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D70" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>11957</v>
+        <v>11954</v>
       </c>
       <c r="B71" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D71" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>11958</v>
+        <v>11955</v>
       </c>
       <c r="B72" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>11961</v>
+        <v>11957</v>
       </c>
       <c r="B73" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>11963</v>
+        <v>11958</v>
       </c>
       <c r="B74" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D74" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>11967</v>
+        <v>11961</v>
       </c>
       <c r="B75" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D75" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>11968</v>
+        <v>11963</v>
       </c>
       <c r="B76" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C76" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D76" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>11971</v>
+        <v>11967</v>
       </c>
       <c r="B77" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D77" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>11976</v>
+        <v>11968</v>
       </c>
       <c r="B78" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D78" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>11977</v>
+        <v>11971</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D79" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>11978</v>
+        <v>11976</v>
       </c>
       <c r="B80" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D80" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>11980</v>
+        <v>11977</v>
       </c>
       <c r="B81" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D81" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>11001</v>
+        <v>11978</v>
       </c>
       <c r="B82" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D82" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>11003</v>
+        <v>11980</v>
       </c>
       <c r="B83" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D83" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>11010</v>
+        <v>11746</v>
       </c>
       <c r="B84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D84" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>11030</v>
+        <v>11747</v>
       </c>
       <c r="B85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D85" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>11050</v>
+        <v>11741</v>
       </c>
       <c r="B86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" t="s">
+        <v>16</v>
+      </c>
+      <c r="D86" t="s">
         <v>30</v>
-      </c>
-      <c r="D86" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>11096</v>
+        <v>11742</v>
       </c>
       <c r="B87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87" t="s">
+        <v>16</v>
+      </c>
+      <c r="D87" t="s">
         <v>30</v>
-      </c>
-      <c r="D87" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>11509</v>
+        <v>11779</v>
       </c>
       <c r="B88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C88" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D88" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>11510</v>
+        <v>11722</v>
       </c>
       <c r="B89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D89" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>11514</v>
+        <v>11749</v>
       </c>
       <c r="B90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D90" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>11516</v>
+        <v>11580</v>
       </c>
       <c r="B91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D91" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>11518</v>
+        <v>11581</v>
       </c>
       <c r="B92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C92" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D92" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>11520</v>
+        <v>11705</v>
       </c>
       <c r="B93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C93" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D93" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>11542</v>
+        <v>11715</v>
       </c>
       <c r="B94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D94" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>11545</v>
+        <v>11716</v>
       </c>
       <c r="B95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D95" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>11548</v>
+        <v>11769</v>
       </c>
       <c r="B96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C96" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D96" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>11550</v>
+        <v>11772</v>
       </c>
       <c r="B97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D97" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>11552</v>
+        <v>11782</v>
       </c>
       <c r="B98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D98" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>11553</v>
+        <v>11796</v>
       </c>
       <c r="B99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D99" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>11554</v>
+        <v>11550</v>
       </c>
       <c r="B100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D100" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>11557</v>
+        <v>11554</v>
       </c>
       <c r="B101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D101" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>11558</v>
+        <v>11510</v>
       </c>
       <c r="B102" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C102" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D102" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>11559</v>
+        <v>11553</v>
       </c>
       <c r="B103" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C103" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D103" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>11560</v>
+        <v>11565</v>
       </c>
       <c r="B104" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C104" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D104" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>11561</v>
+        <v>11575</v>
       </c>
       <c r="B105" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C105" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D105" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>11563</v>
+        <v>11003</v>
       </c>
       <c r="B106" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C106" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D106" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>11565</v>
+        <v>11010</v>
       </c>
       <c r="B107" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D107" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>11568</v>
+        <v>11552</v>
       </c>
       <c r="B108" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D108" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>11570</v>
+        <v>11755</v>
       </c>
       <c r="B109" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C109" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D109" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>11572</v>
+        <v>11766</v>
       </c>
       <c r="B110" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C110" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D110" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>11575</v>
+        <v>11767</v>
       </c>
       <c r="B111" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C111" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D111" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>11576</v>
+        <v>11780</v>
       </c>
       <c r="B112" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C112" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D112" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>11577</v>
+        <v>11096</v>
       </c>
       <c r="B113" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C113" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D113" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>11579</v>
+        <v>11516</v>
       </c>
       <c r="B114" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C114" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D114" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>11580</v>
+        <v>11557</v>
       </c>
       <c r="B115" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C115" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D115" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>11581</v>
+        <v>11559</v>
       </c>
       <c r="B116" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C116" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D116" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>11590</v>
+        <v>11598</v>
       </c>
       <c r="B117" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D117" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>11598</v>
+        <v>11706</v>
       </c>
       <c r="B118" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C118" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D118" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>11705</v>
+        <v>11718</v>
       </c>
       <c r="B119" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C119" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D119" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>11706</v>
+        <v>11727</v>
       </c>
       <c r="B120" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C120" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D120" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>11709</v>
+        <v>11738</v>
       </c>
       <c r="B121" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C121" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D121" t="s">
         <v>8</v>
@@ -2218,478 +2240,478 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>11714</v>
+        <v>11753</v>
       </c>
       <c r="B122" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C122" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D122" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>11715</v>
+        <v>11763</v>
       </c>
       <c r="B123" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C123" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D123" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>11716</v>
+        <v>11784</v>
       </c>
       <c r="B124" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C124" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D124" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>11718</v>
+        <v>11801</v>
       </c>
       <c r="B125" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C125" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D125" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>11720</v>
+        <v>11001</v>
       </c>
       <c r="B126" t="s">
+        <v>0</v>
+      </c>
+      <c r="C126" t="s">
+        <v>16</v>
+      </c>
+      <c r="D126" t="s">
         <v>1</v>
-      </c>
-      <c r="C126" t="s">
-        <v>30</v>
-      </c>
-      <c r="D126" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>11722</v>
+        <v>11030</v>
       </c>
       <c r="B127" t="s">
+        <v>0</v>
+      </c>
+      <c r="C127" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127" t="s">
         <v>1</v>
-      </c>
-      <c r="C127" t="s">
-        <v>30</v>
-      </c>
-      <c r="D127" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>11727</v>
+        <v>11050</v>
       </c>
       <c r="B128" t="s">
+        <v>0</v>
+      </c>
+      <c r="C128" t="s">
+        <v>16</v>
+      </c>
+      <c r="D128" t="s">
         <v>1</v>
-      </c>
-      <c r="C128" t="s">
-        <v>30</v>
-      </c>
-      <c r="D128" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>11732</v>
+        <v>11514</v>
       </c>
       <c r="B129" t="s">
+        <v>0</v>
+      </c>
+      <c r="C129" t="s">
+        <v>16</v>
+      </c>
+      <c r="D129" t="s">
         <v>1</v>
-      </c>
-      <c r="C129" t="s">
-        <v>30</v>
-      </c>
-      <c r="D129" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>11738</v>
+        <v>11568</v>
       </c>
       <c r="B130" t="s">
+        <v>0</v>
+      </c>
+      <c r="C130" t="s">
+        <v>16</v>
+      </c>
+      <c r="D130" t="s">
         <v>1</v>
-      </c>
-      <c r="C130" t="s">
-        <v>30</v>
-      </c>
-      <c r="D130" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>11741</v>
+        <v>11590</v>
       </c>
       <c r="B131" t="s">
+        <v>0</v>
+      </c>
+      <c r="C131" t="s">
+        <v>16</v>
+      </c>
+      <c r="D131" t="s">
         <v>1</v>
-      </c>
-      <c r="C131" t="s">
-        <v>30</v>
-      </c>
-      <c r="D131" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>11742</v>
+        <v>11518</v>
       </c>
       <c r="B132" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C132" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D132" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>11746</v>
+        <v>11520</v>
       </c>
       <c r="B133" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C133" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D133" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>11747</v>
+        <v>11572</v>
       </c>
       <c r="B134" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C134" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D134" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135">
-        <v>11749</v>
+        <v>11577</v>
       </c>
       <c r="B135" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C135" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D135" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136">
-        <v>11753</v>
+        <v>11714</v>
       </c>
       <c r="B136" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C136" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D136" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137">
-        <v>11755</v>
+        <v>11756</v>
       </c>
       <c r="B137" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C137" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D137" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>11756</v>
+        <v>11804</v>
       </c>
       <c r="B138" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C138" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D138" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>11763</v>
+        <v>11542</v>
       </c>
       <c r="B139" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C139" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D139" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>11765</v>
+        <v>11545</v>
       </c>
       <c r="B140" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C140" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D140" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>11766</v>
+        <v>11548</v>
       </c>
       <c r="B141" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C141" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D141" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142">
-        <v>11767</v>
+        <v>11560</v>
       </c>
       <c r="B142" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C142" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D142" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>11769</v>
+        <v>11576</v>
       </c>
       <c r="B143" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C143" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D143" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144">
-        <v>11771</v>
+        <v>11579</v>
       </c>
       <c r="B144" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C144" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D144" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145">
-        <v>11772</v>
+        <v>11709</v>
       </c>
       <c r="B145" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C145" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D145" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>11779</v>
+        <v>11732</v>
       </c>
       <c r="B146" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C146" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D146" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>11780</v>
+        <v>11765</v>
       </c>
       <c r="B147" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C147" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D147" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>11782</v>
+        <v>11771</v>
       </c>
       <c r="B148" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C148" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D148" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>11784</v>
+        <v>11791</v>
       </c>
       <c r="B149" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C149" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D149" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150">
-        <v>11791</v>
+        <v>11797</v>
       </c>
       <c r="B150" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C150" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D150" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151">
-        <v>11796</v>
+        <v>11509</v>
       </c>
       <c r="B151" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C151" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D151" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>11797</v>
+        <v>11558</v>
       </c>
       <c r="B152" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C152" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D152" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153">
-        <v>11801</v>
+        <v>11561</v>
       </c>
       <c r="B153" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C153" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D153" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>11803</v>
+        <v>11563</v>
       </c>
       <c r="B154" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C154" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D154" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>11804</v>
+        <v>11570</v>
       </c>
       <c r="B155" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C155" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D155" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -2697,13 +2719,13 @@
         <v>117</v>
       </c>
       <c r="B156" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C156" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D156" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -2711,18 +2733,18 @@
         <v>11022</v>
       </c>
       <c r="B157" t="s">
+        <v>0</v>
+      </c>
+      <c r="C157" t="s">
+        <v>18</v>
+      </c>
+      <c r="D157" t="s">
         <v>1</v>
-      </c>
-      <c r="C157" t="s">
-        <v>29</v>
-      </c>
-      <c r="D157" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D157">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated type order 50 for CBATT1 from CBATW1, new date will now always be monday
</commit_message>
<xml_diff>
--- a/Zips by Address File Group.xlsx
+++ b/Zips by Address File Group.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimelj/WebDev/CBA/mailApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DF749B-4552-D840-BC57-1DC47618E1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E42FEA-5729-9849-8D44-A1B95B3AFB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{FF0AFF27-4EB4-4517-B714-952991B7B0BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="32">
   <si>
     <t>DDU</t>
   </si>
@@ -125,25 +125,13 @@
     <t>CBAM9</t>
   </si>
   <si>
-    <t>CBAMT1-1</t>
-  </si>
-  <si>
-    <t>CBAMT1-2</t>
-  </si>
-  <si>
-    <t>CBAMT1-3</t>
-  </si>
-  <si>
-    <t>CBAMT1-4</t>
-  </si>
-  <si>
-    <t>CBAMT1-5</t>
-  </si>
-  <si>
     <t>CBAT11</t>
   </si>
   <si>
     <t>CBAT12</t>
+  </si>
+  <si>
+    <t>CBATT1</t>
   </si>
 </sst>
 </file>
@@ -185,17 +173,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -538,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC217B0-B495-4842-AF2B-3B0E925991E5}">
   <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1717,7 +1695,7 @@
         <v>16</v>
       </c>
       <c r="D84" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -1731,7 +1709,7 @@
         <v>16</v>
       </c>
       <c r="D85" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -1745,7 +1723,7 @@
         <v>16</v>
       </c>
       <c r="D86" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -1759,7 +1737,7 @@
         <v>16</v>
       </c>
       <c r="D87" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -1787,7 +1765,7 @@
         <v>16</v>
       </c>
       <c r="D89" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -1801,7 +1779,7 @@
         <v>16</v>
       </c>
       <c r="D90" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -1815,7 +1793,7 @@
         <v>16</v>
       </c>
       <c r="D91" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -1829,7 +1807,7 @@
         <v>16</v>
       </c>
       <c r="D92" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -1969,7 +1947,7 @@
         <v>16</v>
       </c>
       <c r="D102" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -1983,7 +1961,7 @@
         <v>16</v>
       </c>
       <c r="D103" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -1997,7 +1975,7 @@
         <v>16</v>
       </c>
       <c r="D104" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2011,7 +1989,7 @@
         <v>16</v>
       </c>
       <c r="D105" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2025,7 +2003,7 @@
         <v>16</v>
       </c>
       <c r="D106" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2039,7 +2017,7 @@
         <v>16</v>
       </c>
       <c r="D107" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2053,7 +2031,7 @@
         <v>16</v>
       </c>
       <c r="D108" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2744,7 +2722,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D157">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updating capstone date and other changes
</commit_message>
<xml_diff>
--- a/Zips by Address File Group.xlsx
+++ b/Zips by Address File Group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimelj/WebDev/CBA/mailApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E42FEA-5729-9849-8D44-A1B95B3AFB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F32145-566B-F74A-A291-FE82756C457B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{FF0AFF27-4EB4-4517-B714-952991B7B0BD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{FF0AFF27-4EB4-4517-B714-952991B7B0BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="9" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>CBAT1</t>
   </si>
   <si>
-    <t>CBAT99</t>
-  </si>
-  <si>
     <t>SCF</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>CBATT1</t>
+  </si>
+  <si>
+    <t>CBAM99</t>
   </si>
 </sst>
 </file>
@@ -516,24 +516,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC217B0-B495-4842-AF2B-3B0E925991E5}">
   <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D30"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -544,10 +544,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -558,10 +558,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -572,10 +572,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -586,10 +586,10 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -600,10 +600,10 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -614,10 +614,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -628,10 +628,10 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -642,10 +642,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -656,10 +656,10 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -670,10 +670,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -684,10 +684,10 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -698,10 +698,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -712,10 +712,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -726,10 +726,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -740,10 +740,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -754,10 +754,10 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -768,10 +768,10 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -782,10 +782,10 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -796,10 +796,10 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -810,10 +810,10 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -824,10 +824,10 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -838,10 +838,10 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
         <v>18</v>
-      </c>
-      <c r="D23" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -852,10 +852,10 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
         <v>18</v>
-      </c>
-      <c r="D24" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -866,10 +866,10 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
         <v>18</v>
-      </c>
-      <c r="D25" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -880,10 +880,10 @@
         <v>0</v>
       </c>
       <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
         <v>18</v>
-      </c>
-      <c r="D26" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -894,10 +894,10 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
         <v>18</v>
-      </c>
-      <c r="D27" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -908,10 +908,10 @@
         <v>0</v>
       </c>
       <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
         <v>18</v>
-      </c>
-      <c r="D28" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -922,10 +922,10 @@
         <v>0</v>
       </c>
       <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
         <v>18</v>
-      </c>
-      <c r="D29" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -936,10 +936,10 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
         <v>18</v>
-      </c>
-      <c r="D30" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -950,10 +950,10 @@
         <v>0</v>
       </c>
       <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
         <v>18</v>
-      </c>
-      <c r="D31" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -964,10 +964,10 @@
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -978,10 +978,10 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -992,10 +992,10 @@
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1006,10 +1006,10 @@
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1020,10 +1020,10 @@
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1034,10 +1034,10 @@
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1048,10 +1048,10 @@
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1062,10 +1062,10 @@
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1076,10 +1076,10 @@
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1090,10 +1090,10 @@
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1104,10 +1104,10 @@
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1118,10 +1118,10 @@
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1132,10 +1132,10 @@
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1146,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1160,10 +1160,10 @@
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1171,13 +1171,13 @@
         <v>11713</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1185,13 +1185,13 @@
         <v>11719</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1199,13 +1199,13 @@
         <v>11764</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1213,13 +1213,13 @@
         <v>11778</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1227,13 +1227,13 @@
         <v>11786</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1241,13 +1241,13 @@
         <v>11789</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1255,13 +1255,13 @@
         <v>11792</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D53" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1269,13 +1269,13 @@
         <v>11901</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1283,13 +1283,13 @@
         <v>11933</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1297,13 +1297,13 @@
         <v>11934</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1311,13 +1311,13 @@
         <v>11935</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D57" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1325,13 +1325,13 @@
         <v>11937</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D58" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1339,13 +1339,13 @@
         <v>11939</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D59" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1353,13 +1353,13 @@
         <v>11940</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D60" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1367,13 +1367,13 @@
         <v>11941</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1381,13 +1381,13 @@
         <v>11942</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1395,13 +1395,13 @@
         <v>11944</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1409,13 +1409,13 @@
         <v>11946</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D64" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1423,13 +1423,13 @@
         <v>11948</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D65" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1437,13 +1437,13 @@
         <v>11949</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D66" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1451,13 +1451,13 @@
         <v>11950</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D67" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1465,13 +1465,13 @@
         <v>11951</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D68" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1479,13 +1479,13 @@
         <v>11952</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D69" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1493,13 +1493,13 @@
         <v>11953</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D70" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1507,13 +1507,13 @@
         <v>11954</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D71" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1521,13 +1521,13 @@
         <v>11955</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D72" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1535,13 +1535,13 @@
         <v>11957</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D73" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1549,13 +1549,13 @@
         <v>11958</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D74" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1563,13 +1563,13 @@
         <v>11961</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D75" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1577,13 +1577,13 @@
         <v>11963</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D76" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -1591,13 +1591,13 @@
         <v>11967</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D77" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -1605,13 +1605,13 @@
         <v>11968</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D78" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -1619,13 +1619,13 @@
         <v>11971</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D79" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -1633,13 +1633,13 @@
         <v>11976</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D80" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -1647,13 +1647,13 @@
         <v>11977</v>
       </c>
       <c r="B81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D81" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -1661,13 +1661,13 @@
         <v>11978</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D82" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -1675,13 +1675,13 @@
         <v>11980</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D83" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -1692,10 +1692,10 @@
         <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D84" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -1706,10 +1706,10 @@
         <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D85" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -1720,10 +1720,10 @@
         <v>0</v>
       </c>
       <c r="C86" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -1734,10 +1734,10 @@
         <v>0</v>
       </c>
       <c r="C87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D87" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -1748,10 +1748,10 @@
         <v>0</v>
       </c>
       <c r="C88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D88" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -1762,10 +1762,10 @@
         <v>0</v>
       </c>
       <c r="C89" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D89" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -1776,10 +1776,10 @@
         <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D90" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -1790,10 +1790,10 @@
         <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D91" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -1804,10 +1804,10 @@
         <v>0</v>
       </c>
       <c r="C92" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D92" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -1818,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="C93" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D93" t="s">
         <v>5</v>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="C94" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D94" t="s">
         <v>5</v>
@@ -1846,7 +1846,7 @@
         <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D95" t="s">
         <v>5</v>
@@ -1860,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="C96" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D96" t="s">
         <v>5</v>
@@ -1874,7 +1874,7 @@
         <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D97" t="s">
         <v>5</v>
@@ -1888,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="C98" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D98" t="s">
         <v>5</v>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D99" t="s">
         <v>5</v>
@@ -1916,10 +1916,10 @@
         <v>0</v>
       </c>
       <c r="C100" t="s">
+        <v>15</v>
+      </c>
+      <c r="D100" t="s">
         <v>16</v>
-      </c>
-      <c r="D100" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -1930,10 +1930,10 @@
         <v>0</v>
       </c>
       <c r="C101" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D101" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -1944,10 +1944,10 @@
         <v>0</v>
       </c>
       <c r="C102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D102" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -1958,10 +1958,10 @@
         <v>0</v>
       </c>
       <c r="C103" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D103" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -1972,10 +1972,10 @@
         <v>0</v>
       </c>
       <c r="C104" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D104" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -1986,10 +1986,10 @@
         <v>0</v>
       </c>
       <c r="C105" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D105" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2000,10 +2000,10 @@
         <v>0</v>
       </c>
       <c r="C106" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D106" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2014,10 +2014,10 @@
         <v>0</v>
       </c>
       <c r="C107" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D107" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2028,10 +2028,10 @@
         <v>0</v>
       </c>
       <c r="C108" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D108" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2042,10 +2042,10 @@
         <v>0</v>
       </c>
       <c r="C109" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D109" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2056,10 +2056,10 @@
         <v>0</v>
       </c>
       <c r="C110" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D110" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2070,10 +2070,10 @@
         <v>0</v>
       </c>
       <c r="C111" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D111" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -2084,10 +2084,10 @@
         <v>0</v>
       </c>
       <c r="C112" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2098,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="C113" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D113" t="s">
         <v>3</v>
@@ -2112,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="C114" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D114" t="s">
         <v>3</v>
@@ -2126,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="C115" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D115" t="s">
         <v>3</v>
@@ -2140,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="C116" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D116" t="s">
         <v>3</v>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="C117" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D117" t="s">
         <v>3</v>
@@ -2168,7 +2168,7 @@
         <v>0</v>
       </c>
       <c r="C118" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D118" t="s">
         <v>3</v>
@@ -2182,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="C119" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D119" t="s">
         <v>3</v>
@@ -2196,10 +2196,10 @@
         <v>0</v>
       </c>
       <c r="C120" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D120" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -2210,10 +2210,10 @@
         <v>0</v>
       </c>
       <c r="C121" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D121" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -2224,10 +2224,10 @@
         <v>0</v>
       </c>
       <c r="C122" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D122" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -2238,10 +2238,10 @@
         <v>0</v>
       </c>
       <c r="C123" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D123" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -2252,10 +2252,10 @@
         <v>0</v>
       </c>
       <c r="C124" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D124" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -2266,10 +2266,10 @@
         <v>0</v>
       </c>
       <c r="C125" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D125" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -2280,7 +2280,7 @@
         <v>0</v>
       </c>
       <c r="C126" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D126" t="s">
         <v>1</v>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="C127" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D127" t="s">
         <v>1</v>
@@ -2308,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="C128" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D128" t="s">
         <v>1</v>
@@ -2322,7 +2322,7 @@
         <v>0</v>
       </c>
       <c r="C129" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D129" t="s">
         <v>1</v>
@@ -2336,7 +2336,7 @@
         <v>0</v>
       </c>
       <c r="C130" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D130" t="s">
         <v>1</v>
@@ -2350,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="C131" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D131" t="s">
         <v>1</v>
@@ -2364,10 +2364,10 @@
         <v>0</v>
       </c>
       <c r="C132" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D132" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -2378,10 +2378,10 @@
         <v>0</v>
       </c>
       <c r="C133" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D133" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -2392,10 +2392,10 @@
         <v>0</v>
       </c>
       <c r="C134" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D134" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -2406,7 +2406,7 @@
         <v>0</v>
       </c>
       <c r="C135" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D135" t="s">
         <v>2</v>
@@ -2420,7 +2420,7 @@
         <v>0</v>
       </c>
       <c r="C136" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D136" t="s">
         <v>2</v>
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="C137" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D137" t="s">
         <v>2</v>
@@ -2448,7 +2448,7 @@
         <v>0</v>
       </c>
       <c r="C138" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D138" t="s">
         <v>2</v>
@@ -2462,7 +2462,7 @@
         <v>0</v>
       </c>
       <c r="C139" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D139" t="s">
         <v>4</v>
@@ -2476,7 +2476,7 @@
         <v>0</v>
       </c>
       <c r="C140" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D140" t="s">
         <v>4</v>
@@ -2490,7 +2490,7 @@
         <v>0</v>
       </c>
       <c r="C141" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D141" t="s">
         <v>4</v>
@@ -2504,7 +2504,7 @@
         <v>0</v>
       </c>
       <c r="C142" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D142" t="s">
         <v>4</v>
@@ -2518,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="C143" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D143" t="s">
         <v>4</v>
@@ -2532,7 +2532,7 @@
         <v>0</v>
       </c>
       <c r="C144" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D144" t="s">
         <v>4</v>
@@ -2546,7 +2546,7 @@
         <v>0</v>
       </c>
       <c r="C145" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D145" t="s">
         <v>4</v>
@@ -2560,7 +2560,7 @@
         <v>0</v>
       </c>
       <c r="C146" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D146" t="s">
         <v>4</v>
@@ -2574,7 +2574,7 @@
         <v>0</v>
       </c>
       <c r="C147" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D147" t="s">
         <v>4</v>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="C148" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D148" t="s">
         <v>4</v>
@@ -2602,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="C149" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D149" t="s">
         <v>4</v>
@@ -2616,7 +2616,7 @@
         <v>0</v>
       </c>
       <c r="C150" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D150" t="s">
         <v>4</v>
@@ -2630,10 +2630,10 @@
         <v>0</v>
       </c>
       <c r="C151" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D151" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -2644,10 +2644,10 @@
         <v>0</v>
       </c>
       <c r="C152" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D152" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -2658,10 +2658,10 @@
         <v>0</v>
       </c>
       <c r="C153" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D153" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -2672,10 +2672,10 @@
         <v>0</v>
       </c>
       <c r="C154" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -2686,10 +2686,10 @@
         <v>0</v>
       </c>
       <c r="C155" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D155" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -2697,13 +2697,13 @@
         <v>117</v>
       </c>
       <c r="B156" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D156" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -2714,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="C157" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D157" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
updating zips by address zip data
</commit_message>
<xml_diff>
--- a/Zips by Address File Group.xlsx
+++ b/Zips by Address File Group.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimelj/WebDev/CBA/mailApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F32145-566B-F74A-A291-FE82756C457B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78622D1-F1D7-5047-99C5-26C4616C65F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{FF0AFF27-4EB4-4517-B714-952991B7B0BD}"/>
   </bookViews>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC217B0-B495-4842-AF2B-3B0E925991E5}">
   <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="I113" sqref="I113"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2717,7 +2717,7 @@
         <v>17</v>
       </c>
       <c r="D157" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating Zips\ by\ Address\ File\ Group.xlsx
</commit_message>
<xml_diff>
--- a/Zips by Address File Group.xlsx
+++ b/Zips by Address File Group.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimelj/WebDev/CBA/mailApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78622D1-F1D7-5047-99C5-26C4616C65F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E3874E-BFB0-7F42-9B13-E95EF08105A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{FF0AFF27-4EB4-4517-B714-952991B7B0BD}"/>
   </bookViews>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC217B0-B495-4842-AF2B-3B0E925991E5}">
   <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D157" sqref="D157"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1751,7 +1751,7 @@
         <v>15</v>
       </c>
       <c r="D88" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>